<commit_message>
free spin login changed feature track
</commit_message>
<xml_diff>
--- a/INT_data.xlsx
+++ b/INT_data.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eiralee/EiraLi-Katalon_API/INT_env/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eiralee/Katalon_Script/SuperWild/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F187A1-26FC-7143-888B-E4448A6FAEE3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742D2346-2703-9F42-BA95-852C12F2F193}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33020" yWindow="-2300" windowWidth="28060" windowHeight="17100" xr2:uid="{4ABBE822-C540-4244-926E-370C7E326042}"/>
+    <workbookView xWindow="28620" yWindow="-2620" windowWidth="29440" windowHeight="16940" xr2:uid="{4ABBE822-C540-4244-926E-370C7E326042}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="ref" sheetId="2" r:id="rId2"/>
     <sheet name="工作表1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="73">
   <si>
     <t>partner</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -236,14 +236,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2019-07-17T00:00:00Z</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019-07-17T23:59:00Z</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>bbin_int_0001</t>
   </si>
   <si>
@@ -286,6 +278,18 @@
   </si>
   <si>
     <t>nurgs.3655oule.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>krug.3655oule.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-08-22T00:00:00Z</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019-08-22T23:59:00Z</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -804,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670E70B4-D18C-8A41-9D76-6A8C3B916D59}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26"/>
@@ -868,7 +872,7 @@
         <v>53</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1" ht="20">
@@ -882,28 +886,28 @@
         <v>13</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>55</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="L2" s="12" t="s">
         <v>43</v>
@@ -912,7 +916,7 @@
         <v>54</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="2" customFormat="1" ht="20">
@@ -926,28 +930,28 @@
         <v>10</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>55</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="L3" s="12" t="s">
         <v>43</v>
@@ -956,7 +960,7 @@
         <v>54</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="2" customFormat="1" ht="20">
@@ -970,28 +974,28 @@
         <v>16</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>55</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="L4" s="12" t="s">
         <v>43</v>
@@ -1000,7 +1004,7 @@
         <v>54</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="2" customFormat="1" ht="20">
@@ -1014,28 +1018,28 @@
         <v>19</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>55</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="L5" s="12" t="s">
         <v>43</v>
@@ -1044,7 +1048,7 @@
         <v>54</v>
       </c>
       <c r="N5" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="2" customFormat="1" ht="20">
@@ -1058,28 +1062,28 @@
         <v>22</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>55</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="L6" s="12" t="s">
         <v>43</v>
@@ -1088,7 +1092,7 @@
         <v>54</v>
       </c>
       <c r="N6" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="2" customFormat="1" ht="20">
@@ -1102,28 +1106,28 @@
         <v>24</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>55</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="L7" s="12" t="s">
         <v>43</v>
@@ -1132,7 +1136,7 @@
         <v>54</v>
       </c>
       <c r="N7" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="2" customFormat="1" ht="20">
@@ -1146,28 +1150,28 @@
         <v>27</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>55</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="L8" s="12" t="s">
         <v>43</v>
@@ -1176,7 +1180,7 @@
         <v>54</v>
       </c>
       <c r="N8" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="2" customFormat="1" ht="20">
@@ -1190,28 +1194,28 @@
         <v>30</v>
       </c>
       <c r="D9" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>55</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="L9" s="12" t="s">
         <v>43</v>
@@ -1220,7 +1224,7 @@
         <v>54</v>
       </c>
       <c r="N9" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="2" customFormat="1" ht="20">
@@ -1234,28 +1238,28 @@
         <v>33</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>55</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="L10" s="12" t="s">
         <v>43</v>
@@ -1264,7 +1268,7 @@
         <v>54</v>
       </c>
       <c r="N10" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="2" customFormat="1" ht="20"/>

</xml_diff>